<commit_message>
updated basic formulas sheet
</commit_message>
<xml_diff>
--- a/batch_03/excel/Basic_formulas.xlsx
+++ b/batch_03/excel/Basic_formulas.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\TrainerDoc\Programming\data_analytics\batch_03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9E004D-FADC-467C-9ECB-14774785920C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Math Formulas" sheetId="4" r:id="rId1"/>
-    <sheet name="Text Functins" sheetId="1" r:id="rId2"/>
-    <sheet name="Logical Functions" sheetId="3" r:id="rId3"/>
-    <sheet name="date and Time Functions" sheetId="2" r:id="rId4"/>
+    <sheet name="date and Time Functions" sheetId="2" r:id="rId2"/>
+    <sheet name="Text Functins" sheetId="1" r:id="rId3"/>
+    <sheet name="Logical Functions" sheetId="3" r:id="rId4"/>
     <sheet name="Statistical Functions" sheetId="5" r:id="rId5"/>
     <sheet name="Lookup (V and H _Lookup) " sheetId="6" r:id="rId6"/>
     <sheet name="Reference Functions" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="191">
   <si>
     <t>CONCATENATE(), TEXT(), LEFT(), RIGHT(), MID(), LEN(), TRIM(), UPPER(), LOWER(), PROPER(), REPT(), SUBSTITUTE(), FIND(), SEARCH()</t>
   </si>
@@ -261,33 +262,12 @@
     <t>=TIME(2,30,30)</t>
   </si>
   <si>
-    <t>=DATEDIF(F4,G4,"Y")</t>
-  </si>
-  <si>
     <t>=NOW()</t>
   </si>
   <si>
     <t>=TODAY()</t>
   </si>
   <si>
-    <t>=DATE(2020,12,10)</t>
-  </si>
-  <si>
-    <t>=YEAR(G4)</t>
-  </si>
-  <si>
-    <t>=DAY(G4)</t>
-  </si>
-  <si>
-    <t>=HOUR(H4)</t>
-  </si>
-  <si>
-    <t>=MINUTE(H4)</t>
-  </si>
-  <si>
-    <t>=SECOND(H4)</t>
-  </si>
-  <si>
     <t>Value1</t>
   </si>
   <si>
@@ -411,27 +391,9 @@
     <t>Function Name</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>average</t>
-  </si>
-  <si>
-    <t>multiplication | Product</t>
-  </si>
-  <si>
     <t>=LEN(A2)</t>
   </si>
   <si>
-    <t>round()</t>
-  </si>
-  <si>
-    <t>celing()</t>
-  </si>
-  <si>
-    <t>roundup()</t>
-  </si>
-  <si>
     <t>rand()</t>
   </si>
   <si>
@@ -441,9 +403,6 @@
     <t>lower()</t>
   </si>
   <si>
-    <t>12.12.2007</t>
-  </si>
-  <si>
     <t>AVERAGE(), MEDIAN(), MODE(), COUNT(), COUNTA(), COUNTIF(), COUNTIFS(), MAX(), MIN(), STDEV(), VAR()</t>
   </si>
   <si>
@@ -543,12 +502,6 @@
     <t>=COUNT(A2:B2)</t>
   </si>
   <si>
-    <t>dsd</t>
-  </si>
-  <si>
-    <t>gfgf</t>
-  </si>
-  <si>
     <t>=COUNTA(A2:B2)</t>
   </si>
   <si>
@@ -601,12 +554,66 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>=AVERAGE(A2:B2)</t>
+  </si>
+  <si>
+    <t>=SUM(A2:B2)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>=ROUND(L2,0)</t>
+  </si>
+  <si>
+    <t>=CEILING(L2,1)</t>
+  </si>
+  <si>
+    <t>=ROUNDUP(L2,0)</t>
+  </si>
+  <si>
+    <t>=ROUNDDOWN(L2,0)</t>
+  </si>
+  <si>
+    <t>=YEAR(E6)</t>
+  </si>
+  <si>
+    <t>=MONTH(E6)</t>
+  </si>
+  <si>
+    <t>=DAY(E6)</t>
+  </si>
+  <si>
+    <t>=DATE(2022,7,22)</t>
+  </si>
+  <si>
+    <t>=DATEDIF(D6,E6,"Y")</t>
+  </si>
+  <si>
+    <t>=DATEDIF(D6,E6,"M")</t>
+  </si>
+  <si>
+    <t>=DATEDIF(D6,E6,"D")</t>
+  </si>
+  <si>
+    <t>=SECOND(D16)</t>
+  </si>
+  <si>
+    <t>=MINUTE(D16)</t>
+  </si>
+  <si>
+    <t>=HOUR(D16)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -673,7 +680,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -705,13 +712,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -720,14 +738,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -756,7 +774,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -766,9 +784,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -785,7 +805,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -793,6 +813,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1073,1318 +1102,767 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="M1" s="6" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="N1" t="s">
-        <v>130</v>
-      </c>
-      <c r="O1" t="s">
-        <v>131</v>
-      </c>
-      <c r="P1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="R1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+      <c r="H1" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="40">
         <v>333</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="40">
         <v>0</v>
       </c>
-      <c r="C2">
-        <f>SUM(A2:B2,F12:F13,H12:K12)</f>
-        <v>349</v>
-      </c>
-      <c r="D2">
-        <f>A2*B2</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="C2" s="21">
+        <f>SUM(A2:B2)</f>
+        <v>333</v>
+      </c>
+      <c r="D2" s="21">
         <f>PRODUCT(A2:B2)</f>
         <v>0</v>
       </c>
-      <c r="F2" t="e">
+      <c r="E2" s="21" t="e">
         <f>QUOTIENT(A2,B2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G2" t="e">
-        <f t="shared" ref="G2:G13" si="0">MOD(A2,B2)</f>
+      <c r="F2" s="21" t="e">
+        <f>MOD(A2,B2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H11" si="1">AVERAGE(A2:B2)</f>
+      <c r="G2" s="21">
+        <f>AVERAGE(A2:B2)</f>
         <v>166.5</v>
       </c>
-      <c r="I2">
+      <c r="H2" s="21">
         <f>COUNT(A2:B2)</f>
         <v>2</v>
       </c>
-      <c r="J2">
+      <c r="I2" s="21">
         <f>COUNTA(A2:B2)</f>
         <v>2</v>
       </c>
-      <c r="K2">
+      <c r="J2" s="21">
         <f>LEN(A2)</f>
         <v>3</v>
       </c>
-      <c r="L2">
-        <f>POWER(A2,2)</f>
-        <v>110889</v>
-      </c>
-      <c r="M2">
-        <f>SQRT(A2)</f>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N2">
-        <f>ROUND(M2,0)</f>
-        <v>18</v>
-      </c>
-      <c r="O2">
-        <f>CEILING(M2,2)</f>
-        <v>20</v>
-      </c>
-      <c r="P2">
-        <f>ROUNDUP(M2,0)</f>
-        <v>19</v>
-      </c>
-      <c r="Q2">
+      <c r="K2" s="21">
+        <f>POWER(H2,J2)</f>
+        <v>8</v>
+      </c>
+      <c r="L2" s="42">
+        <f>SQRT(K2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M2" s="42">
+        <f>ROUND(L2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="N2" s="21">
+        <f>CEILING(L2,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O2" s="42">
+        <f>ROUNDUP(L2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="P2" s="42">
+        <f>ROUNDDOWN(L2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q2" s="21">
         <f ca="1">RAND()</f>
-        <v>0.19238299205424803</v>
-      </c>
-      <c r="R2">
+        <v>0.95869055737930298</v>
+      </c>
+      <c r="R2" s="21">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+        <v>9020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
         <v>11</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="40">
         <v>2</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C22" si="2">SUM(A3:B3)</f>
+      <c r="C3" s="21">
+        <f t="shared" ref="C3:C9" si="0">SUM(A3:B3)</f>
         <v>13</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F7" si="3">QUOTIENT(A3,B3)</f>
+      <c r="D3" s="21">
+        <f t="shared" ref="D3:D9" si="1">PRODUCT(A3:B3)</f>
+        <v>22</v>
+      </c>
+      <c r="E3" s="21">
+        <f t="shared" ref="E3:E9" si="2">QUOTIENT(A3,B3)</f>
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="F3" s="21">
+        <f t="shared" ref="F3:F9" si="3">MOD(A3,B3)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="21">
+        <f t="shared" ref="G3:G9" si="4">AVERAGE(A3:B3)</f>
+        <v>6.5</v>
+      </c>
+      <c r="H3" s="21">
+        <f t="shared" ref="H3:H9" si="5">COUNT(A3:B3)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="21">
+        <f t="shared" ref="I3:I10" si="6">COUNTA(A3:B3)</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="21">
+        <f t="shared" ref="J3:J10" si="7">LEN(A3)</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="21">
+        <f t="shared" ref="K3:K10" si="8">POWER(H3,J3)</f>
+        <v>4</v>
+      </c>
+      <c r="L3" s="42">
+        <f t="shared" ref="L3:L10" si="9">SQRT(K3)</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="42">
+        <f t="shared" ref="M3:M10" si="10">ROUND(L3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="N3" s="21">
+        <f t="shared" ref="N3:N10" si="11">CEILING(L3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="O3" s="42">
+        <f t="shared" ref="O3:O10" si="12">ROUNDUP(L3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="P3" s="42">
+        <f t="shared" ref="P3:P10" si="13">ROUNDDOWN(L3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="Q3" s="21">
+        <f t="shared" ref="Q3:Q10" ca="1" si="14">RAND()</f>
+        <v>0.43734862319250578</v>
+      </c>
+      <c r="R3" s="21">
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>9101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="40">
+        <v>333</v>
+      </c>
+      <c r="B4" s="40">
+        <v>0</v>
+      </c>
+      <c r="C4" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H3">
+        <v>333</v>
+      </c>
+      <c r="D4" s="21">
         <f t="shared" si="1"/>
-        <v>6.5</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I11" si="4">COUNT(A3:B3)</f>
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J22" si="5">COUNTA(A3:B3)</f>
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K22" si="6">LEN(A3)</f>
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <f>POWER(A3,K2)</f>
-        <v>1331</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M26" si="7">SQRT(A3)</f>
-        <v>3.3166247903553998</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N26" si="8">ROUND(M3,2)</f>
-        <v>3.32</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P26" si="9">ROUNDUP(M3,0)</f>
-        <v>4</v>
-      </c>
-      <c r="Q3">
-        <f ca="1">RAND()</f>
-        <v>8.62429937706225E-2</v>
-      </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R26" ca="1" si="10">RANDBETWEEN(1000,9999)</f>
-        <v>5019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <v>333</v>
-      </c>
-      <c r="B4" s="12">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="E4" s="21" t="e">
         <f t="shared" si="2"/>
-        <v>333</v>
-      </c>
-      <c r="F4" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" s="21" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
+      <c r="G4" s="21">
+        <f t="shared" si="4"/>
         <v>166.5</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="K4">
+      <c r="I4" s="21">
         <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J4" s="21">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L26" si="11">POWER(A4,K3)</f>
-        <v>110889</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N4">
+      <c r="K4" s="21">
         <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="L4" s="42">
         <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q4">
-        <f ca="1">RAND()</f>
-        <v>0.37549659708205807</v>
-      </c>
-      <c r="R4">
-        <f t="shared" ca="1" si="10"/>
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M4" s="42">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N4" s="21">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="O4" s="42">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P4" s="42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q4" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.57420508734810982</v>
+      </c>
+      <c r="R4" s="21">
+        <f t="shared" ref="R3:R10" ca="1" si="15">RANDBETWEEN(1000,9999)</f>
+        <v>7405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="40">
         <v>333</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="40">
         <v>45</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="21">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+      <c r="D5" s="21">
+        <f t="shared" si="1"/>
+        <v>14985</v>
+      </c>
+      <c r="E5" s="21">
         <f t="shared" si="2"/>
-        <v>378</v>
-      </c>
-      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="F5" s="21">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
+      <c r="G5" s="21">
+        <f t="shared" si="4"/>
         <v>189</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J5">
+      <c r="H5" s="21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="K5">
+      <c r="I5" s="21">
         <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J5" s="21">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="K5" s="21">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L5" s="42">
+        <f t="shared" si="9"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M5" s="42">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N5" s="21">
         <f t="shared" si="11"/>
-        <v>36926037</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" ref="Q5:Q26" ca="1" si="12">RAND()</f>
-        <v>0.901382427733458</v>
-      </c>
-      <c r="R5">
-        <f t="shared" ca="1" si="10"/>
-        <v>6527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="O5" s="42">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P5" s="42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.14544016788737646</v>
+      </c>
+      <c r="R5" s="21">
+        <f t="shared" ca="1" si="15"/>
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
         <v>333</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="40">
         <v>55</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="21">
+        <f t="shared" si="0"/>
+        <v>388</v>
+      </c>
+      <c r="D6" s="21">
+        <f t="shared" si="1"/>
+        <v>18315</v>
+      </c>
+      <c r="E6" s="21">
         <f t="shared" si="2"/>
-        <v>388</v>
-      </c>
-      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="F6" s="21">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
+      <c r="G6" s="21">
+        <f t="shared" si="4"/>
         <v>194</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J6">
+      <c r="H6" s="21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="K6">
+      <c r="I6" s="21">
         <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J6" s="21">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L6">
+      <c r="K6" s="21">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L6" s="42">
+        <f t="shared" si="9"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M6" s="42">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N6" s="21">
         <f t="shared" si="11"/>
-        <v>36926037</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.59337110472544152</v>
-      </c>
-      <c r="R6">
-        <f t="shared" ca="1" si="10"/>
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+        <v>3</v>
+      </c>
+      <c r="O6" s="42">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P6" s="42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q6" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.71651352700659721</v>
+      </c>
+      <c r="R6" s="21">
+        <f t="shared" ca="1" si="15"/>
+        <v>9735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
         <v>333</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="40">
         <v>65</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="21">
+        <f t="shared" si="0"/>
+        <v>398</v>
+      </c>
+      <c r="D7" s="21">
+        <f t="shared" si="1"/>
+        <v>21645</v>
+      </c>
+      <c r="E7" s="21">
         <f t="shared" si="2"/>
-        <v>398</v>
-      </c>
-      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="21">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
+      <c r="G7" s="21">
+        <f t="shared" si="4"/>
         <v>199</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J7">
+      <c r="H7" s="21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="K7">
+      <c r="I7" s="21">
         <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J7" s="21">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L7">
+      <c r="K7" s="21">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L7" s="42">
+        <f t="shared" si="9"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M7" s="42">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N7" s="21">
         <f t="shared" si="11"/>
-        <v>36926037</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.29015277845392962</v>
-      </c>
-      <c r="R7">
-        <f t="shared" ca="1" si="10"/>
-        <v>2719</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+        <v>3</v>
+      </c>
+      <c r="O7" s="42">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P7" s="42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q7" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.94267330701554053</v>
+      </c>
+      <c r="R7" s="21">
+        <f t="shared" ca="1" si="15"/>
+        <v>5402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
         <v>333</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="40">
         <v>75</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="21">
+        <f t="shared" si="0"/>
+        <v>408</v>
+      </c>
+      <c r="D8" s="21">
+        <f t="shared" si="1"/>
+        <v>24975</v>
+      </c>
+      <c r="E8" s="21">
         <f t="shared" si="2"/>
-        <v>408</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F8" s="21">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
+      <c r="G8" s="21">
+        <f t="shared" si="4"/>
         <v>204</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J8">
+      <c r="H8" s="21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="K8">
+      <c r="I8" s="21">
         <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="J8" s="21">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="L8">
+      <c r="K8" s="21">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L8" s="42">
+        <f t="shared" si="9"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M8" s="42">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N8" s="21">
         <f t="shared" si="11"/>
-        <v>36926037</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" ca="1" si="12"/>
-        <v>1.2095115990674921E-2</v>
-      </c>
-      <c r="R8">
-        <f t="shared" ca="1" si="10"/>
-        <v>2896</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+        <v>3</v>
+      </c>
+      <c r="O8" s="42">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P8" s="42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q8" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.17540611960279573</v>
+      </c>
+      <c r="R8" s="21">
+        <f t="shared" ca="1" si="15"/>
+        <v>6292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
         <v>333</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="40">
         <v>85</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="21">
+        <f t="shared" si="0"/>
+        <v>418</v>
+      </c>
+      <c r="D9" s="21">
+        <f t="shared" si="1"/>
+        <v>28305</v>
+      </c>
+      <c r="E9" s="21">
         <f t="shared" si="2"/>
-        <v>418</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="21">
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
+      <c r="G9" s="21">
+        <f t="shared" si="4"/>
         <v>209</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J9">
+      <c r="H9" s="21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="11"/>
-        <v>36926037</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.57095971936851053</v>
-      </c>
-      <c r="R9">
-        <f t="shared" ca="1" si="10"/>
-        <v>5866</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B10" s="12">
-        <v>95</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-      <c r="G10" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="L10" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M10" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N10" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P10" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.75878012035016884</v>
-      </c>
-      <c r="R10">
-        <f t="shared" ca="1" si="10"/>
-        <v>7098</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
-        <v>333</v>
-      </c>
-      <c r="B11" s="12">
-        <v>105</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="2"/>
-        <v>438</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>219</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="11"/>
-        <v>12296370321</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.84222117507418748</v>
-      </c>
-      <c r="R11">
-        <f t="shared" ca="1" si="10"/>
-        <v>2694</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K12">
+      <c r="I9" s="21">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="L12">
+      <c r="J9" s="21">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K9" s="21">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L9" s="42">
+        <f t="shared" si="9"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="M9" s="42">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="N9" s="21">
         <f t="shared" si="11"/>
-        <v>10648</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" ca="1" si="12"/>
-        <v>6.8908834563663479E-3</v>
-      </c>
-      <c r="R12">
-        <f t="shared" ca="1" si="10"/>
-        <v>2332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+        <v>3</v>
+      </c>
+      <c r="O9" s="42">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="P9" s="42">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="Q9" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.13981685702166113</v>
+      </c>
+      <c r="R9" s="21">
+        <f t="shared" ca="1" si="15"/>
+        <v>5491</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="41">
         <v>22</v>
       </c>
-      <c r="B13" s="12">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K13">
+      <c r="C10" s="21">
+        <f t="shared" ref="C10" si="16">SUM(A10:B10)</f>
+        <v>22</v>
+      </c>
+      <c r="D10" s="21">
+        <f t="shared" ref="D10" si="17">PRODUCT(A10:B10)</f>
+        <v>22</v>
+      </c>
+      <c r="E10" s="21" t="e">
+        <f t="shared" ref="E10" si="18">QUOTIENT(A10,B10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F10" s="21" t="e">
+        <f t="shared" ref="F10" si="19">MOD(A10,B10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" s="21">
+        <f t="shared" ref="G10" si="20">AVERAGE(A10:B10)</f>
+        <v>22</v>
+      </c>
+      <c r="H10" s="21">
+        <f>COUNT(A10:B10)</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="21">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="11"/>
-        <v>484</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.52300600087979587</v>
-      </c>
-      <c r="R13">
-        <f t="shared" ca="1" si="10"/>
-        <v>8279</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
-        <v>22</v>
-      </c>
-      <c r="B14" s="12">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="11"/>
-        <v>484</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.1262211183388362</v>
-      </c>
-      <c r="R14">
-        <f t="shared" ca="1" si="10"/>
-        <v>5579</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
-        <v>22</v>
-      </c>
-      <c r="B15" s="12">
-        <v>12</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="11"/>
-        <v>484</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.49549278636070104</v>
-      </c>
-      <c r="R15">
-        <f t="shared" ca="1" si="10"/>
-        <v>5485</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
-        <v>22</v>
-      </c>
-      <c r="B16" s="12">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="11"/>
-        <v>484</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" ca="1" si="12"/>
-        <v>3.1476734788810856E-2</v>
-      </c>
-      <c r="R16">
-        <f t="shared" ca="1" si="10"/>
-        <v>4902</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
-        <v>22</v>
-      </c>
-      <c r="B17" s="12">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="11"/>
-        <v>484</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.21894267995436323</v>
-      </c>
-      <c r="R17">
-        <f t="shared" ca="1" si="10"/>
-        <v>6755</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="12">
-        <v>22</v>
-      </c>
-      <c r="B18" s="12">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="11"/>
-        <v>484</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="7"/>
-        <v>4.6904157598234297</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="8"/>
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.14835729027389588</v>
-      </c>
-      <c r="R18">
-        <f t="shared" ca="1" si="10"/>
-        <v>2097</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f>SUM(A2:A18)</f>
-        <v>2829</v>
-      </c>
-      <c r="B19">
-        <f>SUM(B2:B18)</f>
-        <v>611</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
-        <v>3440</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="11"/>
-        <v>8003241</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="7"/>
-        <v>53.1883445878888</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="8"/>
-        <v>53.19</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="9"/>
-        <v>54</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" ca="1" si="12"/>
-        <v>8.4073738501228568E-2</v>
-      </c>
-      <c r="R19">
-        <f t="shared" ca="1" si="10"/>
-        <v>8138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f>AVERAGE(A2:A18)</f>
-        <v>176.8125</v>
-      </c>
-      <c r="B20">
-        <f>AVERAGE(B2:B18)</f>
-        <v>35.941176470588232</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
-        <v>212.75367647058823</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="11"/>
-        <v>977353920.04518127</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="7"/>
-        <v>13.2970861469722</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="8"/>
-        <v>13.3</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="9"/>
-        <v>14</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.7841223982581178</v>
-      </c>
-      <c r="R20">
-        <f t="shared" ca="1" si="10"/>
-        <v>5808</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f>COUNT(A2:A18)</f>
-        <v>16</v>
-      </c>
-      <c r="B21">
-        <f>COUNT(B2:B18)</f>
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="11"/>
-        <v>4294967296</v>
-      </c>
-      <c r="M21">
+      <c r="J10" s="21">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N21">
+      <c r="K10" s="21">
         <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="L10" s="42">
         <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.77453556935757928</v>
-      </c>
-      <c r="R21">
-        <f t="shared" ca="1" si="10"/>
-        <v>4327</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f>MAX(A2:A18)</f>
-        <v>333</v>
-      </c>
-      <c r="B22">
-        <f>MAX(B2:B18)</f>
-        <v>105</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="2"/>
-        <v>438</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M10" s="42">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="21">
         <f t="shared" si="11"/>
-        <v>110889</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="7"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="8"/>
-        <v>18.25</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.36473868223062333</v>
-      </c>
-      <c r="R22">
-        <f t="shared" ca="1" si="10"/>
-        <v>1868</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f>MIN(A2:A18)</f>
-        <v>11</v>
-      </c>
-      <c r="B23">
-        <f>MIN(B2:B18)</f>
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="11"/>
-        <v>1331</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="7"/>
-        <v>3.3166247903553998</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="8"/>
-        <v>3.32</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.96256201152241105</v>
-      </c>
-      <c r="R23">
-        <f t="shared" ca="1" si="10"/>
-        <v>7994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F24">
-        <f>COUNT(A2:A18,A25:A26)</f>
-        <v>16</v>
-      </c>
-      <c r="L24" t="e">
-        <f t="shared" si="11"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.11172218085511543</v>
-      </c>
-      <c r="R24">
-        <f t="shared" ca="1" si="10"/>
-        <v>6694</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>170</v>
-      </c>
-      <c r="F25">
-        <f>COUNTA(A2:A18,A25:A26)</f>
-        <v>19</v>
-      </c>
-      <c r="L25" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M25" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N25" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P25" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.42031963699898867</v>
-      </c>
-      <c r="R25">
-        <f t="shared" ca="1" si="10"/>
-        <v>7186</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>170</v>
-      </c>
-      <c r="L26" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M26" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N26" t="e">
-        <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P26" t="e">
-        <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.77979638702882492</v>
-      </c>
-      <c r="R26">
-        <f t="shared" ca="1" si="10"/>
-        <v>6231</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O10" s="42">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="P10" s="42">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="21">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.23187239016639161</v>
+      </c>
+      <c r="R10" s="21">
+        <f t="shared" ca="1" si="15"/>
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="21"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="21"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="21"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R16" s="21"/>
+    </row>
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="21"/>
+    </row>
+    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="21"/>
+    </row>
+    <row r="19" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R19" s="21"/>
+    </row>
+    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="21"/>
+    </row>
+    <row r="21" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R21" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2392,40 +1870,294 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:Z20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D6" s="3">
+        <f>DATE(2022,7,22)</f>
+        <v>44764</v>
+      </c>
+      <c r="E6" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45860</v>
+      </c>
+      <c r="F6">
+        <f>YEAR(D6)</f>
+        <v>2022</v>
+      </c>
+      <c r="G6">
+        <f>MONTH(D6)</f>
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <f>DAY(D6)</f>
+        <v>22</v>
+      </c>
+      <c r="J6">
+        <f ca="1">DATEDIF(D6,E6,"Y")</f>
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f ca="1">DATEDIF(D6,E6,"M")</f>
+        <v>36</v>
+      </c>
+      <c r="L6">
+        <f ca="1">DATEDIF(D6,E6,"D")</f>
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="L9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <f ca="1">NOW()</f>
+        <v>45860.463135763886</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="I10" s="20"/>
+      <c r="L10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+      <c r="I11" s="20"/>
+      <c r="L11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I12" s="20"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E13" s="19"/>
+      <c r="G13" s="4"/>
+      <c r="I13" s="20"/>
+      <c r="L13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="L14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="I15" s="20"/>
+      <c r="L15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D16" s="5">
+        <f>TIME(2,30,30)</f>
+        <v>0.10451388888888889</v>
+      </c>
+      <c r="E16" s="20">
+        <f>HOUR(D16)</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="20">
+        <f>MINUTE(D16)</f>
+        <v>30</v>
+      </c>
+      <c r="G16" s="20">
+        <f>SECOND(D16)</f>
+        <v>30</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="L16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I17" s="20"/>
+      <c r="L17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="I18" s="20"/>
+      <c r="L18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E20" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="A1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC34"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:29" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
@@ -2458,7 +2190,7 @@
       <c r="AB1" s="33"/>
       <c r="AC1" s="33"/>
     </row>
-    <row r="2" spans="1:29" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2491,7 +2223,7 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2547,7 +2279,7 @@
         <v>69</v>
       </c>
       <c r="T3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="U3" t="s">
         <v>70</v>
@@ -2565,7 +2297,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2602,7 +2334,7 @@
       </c>
       <c r="L4" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>02/13/2025</v>
+        <v>07/22/2025</v>
       </c>
       <c r="M4" t="str">
         <f>LEFT(F4,5)</f>
@@ -2642,7 +2374,7 @@
       </c>
       <c r="W4" t="str">
         <f ca="1">SUBSTITUTE(L4,"/","-")</f>
-        <v>02-13-2025</v>
+        <v>07-22-2025</v>
       </c>
       <c r="X4">
         <f>FIND("Trichy",K4)</f>
@@ -2653,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2705,7 +2437,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2749,7 +2481,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2786,7 +2518,7 @@
       </c>
       <c r="L7" s="3">
         <f ca="1">TODAY()</f>
-        <v>45701</v>
+        <v>45860</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
@@ -2797,7 +2529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2841,7 +2573,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2881,7 +2613,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2921,7 +2653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2961,7 +2693,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3001,7 +2733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3041,7 +2773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -3081,7 +2813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -3121,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -3161,7 +2893,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -3201,7 +2933,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -3241,7 +2973,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -3281,7 +3013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -3321,7 +3053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -3361,7 +3093,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -3401,7 +3133,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -3441,7 +3173,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -3477,7 +3209,7 @@
         <v>Chennai_Member</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -3513,7 +3245,7 @@
         <v>karur_Normal</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -3549,7 +3281,7 @@
         <v>karur_Normal</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -3585,7 +3317,7 @@
         <v>Trichy_Normal</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -3621,7 +3353,7 @@
         <v>Trichy_Member</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3657,7 +3389,7 @@
         <v>Trichy_Member</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3693,7 +3425,7 @@
         <v>karur_Normal</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -3729,7 +3461,7 @@
         <v>Trichy_Normal</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -3765,7 +3497,7 @@
         <v>karur_Normal</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -3801,7 +3533,7 @@
         <v>Trichy_Normal</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -3847,8 +3579,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3858,182 +3590,181 @@
       <selection pane="bottomRight" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" customWidth="1"/>
+    <col min="1" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
-    <col min="5" max="5" width="37.5546875" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
-    <col min="7" max="7" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="7" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="O1" s="7"/>
       <c r="P1" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="Q1" s="8"/>
       <c r="S1" s="11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
       <c r="D2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="O2" s="7"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="S2" s="11" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>123</v>
-      </c>
       <c r="S3" s="11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>40</v>
       </c>
@@ -4100,13 +3831,13 @@
         <v>70</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>55</v>
       </c>
@@ -4152,13 +3883,13 @@
         <v>30</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>30</v>
       </c>
@@ -4204,13 +3935,13 @@
         <v>30</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>40</v>
       </c>
@@ -4253,13 +3984,13 @@
         <v>0</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>50</v>
       </c>
@@ -4302,13 +4033,13 @@
         <v>0</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -4327,13 +4058,13 @@
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
       <c r="S9" s="11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -4352,21 +4083,21 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
       <c r="S10" s="11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="T10" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="S11" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T14" t="b">
         <f>FALSE</f>
         <v>0</v>
@@ -4383,404 +4114,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z20"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C5" s="3">
-        <f>DATE(2020,12,10)</f>
-        <v>44175</v>
-      </c>
-      <c r="D5" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45701</v>
-      </c>
-      <c r="E5" s="4">
-        <f ca="1">NOW()</f>
-        <v>45701.618897800923</v>
-      </c>
-      <c r="F5" s="5">
-        <f>TIME(2,30,30)</f>
-        <v>0.10451388888888889</v>
-      </c>
-      <c r="G5">
-        <f ca="1">DATEDIF(C5,D5,"ym")</f>
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <f ca="1">YEAR(D5)</f>
-        <v>2025</v>
-      </c>
-      <c r="I5">
-        <f ca="1">DAY(D5)</f>
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <f ca="1">HOUR(E5)</f>
-        <v>14</v>
-      </c>
-      <c r="K5">
-        <f ca="1">MINUTE(E5)</f>
-        <v>51</v>
-      </c>
-      <c r="L5">
-        <f ca="1">SECOND(E5)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I9" s="20">
-        <v>12</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
-      </c>
-      <c r="K9">
-        <v>2002</v>
-      </c>
-      <c r="L9" s="3">
-        <f>DATE(K9,J9,I9)</f>
-        <v>37602</v>
-      </c>
-      <c r="N9" s="3">
-        <v>37602</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D10" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45701</v>
-      </c>
-      <c r="E10">
-        <f ca="1">YEAR(D10)</f>
-        <v>2025</v>
-      </c>
-      <c r="F10">
-        <f ca="1">MONTH(E10)</f>
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <f ca="1">YEARFRAC(TODAY(),C5)</f>
-        <v>4.1749999999999998</v>
-      </c>
-      <c r="I10" s="20">
-        <v>12</v>
-      </c>
-      <c r="J10">
-        <v>12</v>
-      </c>
-      <c r="K10">
-        <v>2001</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" ref="L10:L18" si="0">DATE(K10,J10,I10)</f>
-        <v>37237</v>
-      </c>
-      <c r="N10" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D11" s="4">
-        <f ca="1">NOW()</f>
-        <v>45701.618897685184</v>
-      </c>
-      <c r="I11" s="20">
-        <v>12</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11">
-        <v>2001</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="0"/>
-        <v>37237</v>
-      </c>
-      <c r="M11">
-        <f>DATEDIF(L11,L13,"Y")</f>
-        <v>800</v>
-      </c>
-      <c r="N11" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I12" s="20"/>
-      <c r="L12" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N12" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E13" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="G13" s="4">
-        <v>45695.616666666669</v>
-      </c>
-      <c r="I13" s="20">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>12</v>
-      </c>
-      <c r="K13">
-        <v>2801</v>
-      </c>
-      <c r="L13" s="3">
-        <f>DATE(K13,J13,I13)</f>
-        <v>329431</v>
-      </c>
-      <c r="N13" s="3">
-        <v>329431</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E14" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45701</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="L14" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E15" s="3">
-        <v>45695</v>
-      </c>
-      <c r="G15" s="4">
-        <f ca="1">NOW()</f>
-        <v>45701.618897685184</v>
-      </c>
-      <c r="I15" s="20">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-      <c r="K15">
-        <v>2009</v>
-      </c>
-      <c r="L15" s="3">
-        <f>DATE(K15,J15,I15)</f>
-        <v>40159</v>
-      </c>
-      <c r="N15" s="3">
-        <v>40159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E16" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="L16" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N16" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="I17" s="20"/>
-      <c r="L17" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N17" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E18" s="3">
-        <v>45695</v>
-      </c>
-      <c r="I18" s="20">
-        <v>12</v>
-      </c>
-      <c r="J18">
-        <v>12</v>
-      </c>
-      <c r="K18">
-        <v>2001</v>
-      </c>
-      <c r="L18" s="3">
-        <f t="shared" si="0"/>
-        <v>37237</v>
-      </c>
-      <c r="N18" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E19" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="L19" t="s">
-        <v>136</v>
-      </c>
-      <c r="N19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E20" s="19">
-        <v>0.6166666666666667</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="A1:T1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -4802,18 +4164,18 @@
       <c r="S1" s="38"/>
       <c r="T1" s="38"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
@@ -4827,7 +4189,7 @@
       <c r="O2" s="37"/>
       <c r="P2" s="37"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
@@ -4845,47 +4207,47 @@
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="23" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="N4" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>155</v>
       </c>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>44</v>
       </c>
@@ -4940,7 +4302,7 @@
         <v>58.799999999999955</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>30</v>
       </c>
@@ -4967,7 +4329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>30</v>
       </c>
@@ -4990,7 +4352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>30</v>
       </c>
@@ -5013,7 +4375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>44</v>
       </c>
@@ -5036,20 +4398,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N11">
         <f>SQRT(N5)</f>
         <v>7.6681158050723228</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B16" s="35"/>
       <c r="C16">
@@ -5072,9 +4434,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17">
@@ -5096,7 +4458,7 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -5115,23 +4477,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B1" s="38" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -5152,18 +4514,18 @@
       <c r="S1" s="38"/>
       <c r="T1" s="38"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
@@ -5182,7 +4544,7 @@
       <c r="S2" s="22"/>
       <c r="T2" s="22"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
@@ -5190,7 +4552,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -5198,7 +4560,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
@@ -5212,7 +4574,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
@@ -5226,15 +4588,15 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="24" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B7" s="12">
         <v>30</v>
@@ -5253,9 +4615,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B8" s="12">
         <v>40</v>
@@ -5264,7 +4626,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E8" s="12">
         <v>33</v>
@@ -5280,9 +4642,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B9" s="12">
         <v>50</v>
@@ -5294,21 +4656,21 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="24" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H9" s="24">
         <f>VLOOKUP(G9,A5:F9,3)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>13</v>
@@ -5317,24 +4679,24 @@
         <v>34</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B17" s="12">
         <v>40</v>
@@ -5352,16 +4714,16 @@
         <v>50</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="H17" s="25">
         <f>HLOOKUP(G17,A16:F26,2,)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B18" s="12">
         <v>0</v>
@@ -5386,16 +4748,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -5404,7 +4766,7 @@
       </c>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -5426,26 +4788,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C1" s="39" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -5464,9 +4826,9 @@
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D2" s="35" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
@@ -5481,7 +4843,7 @@
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
@@ -5492,156 +4854,108 @@
         <v>19</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" s="31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="31">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="30">
         <v>25</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5">
         <f>INDEX(A4:C21, 3,2)</f>
         <v>30</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5">
         <f>MATCH("Sarah", A4:A7, 0)</f>
         <v>3</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5">
         <f ca="1">INDIRECT("B5")</f>
         <v>25</v>
       </c>
-      <c r="G5" s="30" t="str">
+      <c r="G5" t="str">
         <f ca="1">OFFSET(B5, 2, 1)</f>
         <v>male</v>
       </c>
-      <c r="H5" s="30" t="str">
+      <c r="H5" t="str">
         <f>CHOOSE(2, A5,A6,A7)</f>
         <v>Sarah</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5">
         <f>ROW(C7)</f>
         <v>7</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5">
         <f>COLUMN(C7)</f>
         <v>3</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="31">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="30">
         <v>30</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30">
+      <c r="E6">
         <f>MATCH(27, B4:B7, 1)</f>
         <v>2</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6">
         <f>B5</f>
         <v>25</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B7" s="27">
         <v>35</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f>A5</f>
         <v>John</v>
@@ -5658,16 +4972,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'Reference Functions'!A4</f>
         <v>Name</v>
@@ -5677,7 +4991,7 @@
         <v>Gender</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Reference Functions'!A5</f>
         <v>John</v>
@@ -5687,7 +5001,7 @@
         <v>Male</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Reference Functions'!A6</f>
         <v>Sarah</v>
@@ -5697,7 +5011,7 @@
         <v>Female</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Reference Functions'!A7</f>
         <v>Mike</v>
@@ -5707,7 +5021,7 @@
         <v>male</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>'Reference Functions'!A8</f>
         <v>0</v>
@@ -5717,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>'Reference Functions'!A9</f>
         <v>0</v>
@@ -5727,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>'Reference Functions'!A10</f>
         <v>0</v>
@@ -5737,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>'Reference Functions'!A11</f>
         <v>0</v>
@@ -5747,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>'Reference Functions'!A12</f>
         <v>0</v>
@@ -5757,7 +5071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>'Reference Functions'!A13</f>
         <v>0</v>
@@ -5767,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>'Reference Functions'!A14</f>
         <v>0</v>

</xml_diff>

<commit_message>
updated the basic formulas sheet
</commit_message>
<xml_diff>
--- a/batch_03/excel/Basic_formulas.xlsx
+++ b/batch_03/excel/Basic_formulas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TrainerDoc\Programming\data_analytics\batch_03\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF34DA0-1F7B-4685-904A-1DDBFDEC23CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D064DCB-F9D9-4574-AEC4-549CBD95DE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Math Formulas" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="Reference Functions" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Logical Functions'!$A$5:$G$8</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="203">
   <si>
     <t>CONCATENATE(), TEXT(), LEFT(), RIGHT(), MID(), LEN(), TRIM(), UPPER(), LOWER(), PROPER(), REPT(), SUBSTITUTE(), FIND(), SEARCH()</t>
   </si>
@@ -610,6 +613,39 @@
   <si>
     <t>Customer ID creation Randomly
 =UPPER(CONCATENATE("CUST",LEFT(A4,2),"BR",B4,"LOC",LEFT(C4,3),RANDBETWEEN(1000,9999)))</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ragu</t>
+  </si>
+  <si>
+    <t>ravi</t>
+  </si>
+  <si>
+    <t>raju</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>ragav</t>
+  </si>
+  <si>
+    <t>fees</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>python</t>
   </si>
 </sst>
 </file>
@@ -769,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -841,13 +877,31 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -864,21 +918,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1311,11 +1350,11 @@
       </c>
       <c r="Q2" s="21">
         <f ca="1">RAND()</f>
-        <v>0.52349882640039946</v>
+        <v>0.72901728750663719</v>
       </c>
       <c r="R2" s="21">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>2272</v>
+        <v>5953</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1383,11 +1422,11 @@
       </c>
       <c r="Q3" s="21">
         <f t="shared" ref="Q3:Q10" ca="1" si="14">RAND()</f>
-        <v>0.64080971851774204</v>
+        <v>0.66559471269613701</v>
       </c>
       <c r="R3" s="21">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>5194</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1455,11 +1494,11 @@
       </c>
       <c r="Q4" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.58211776566942885</v>
+        <v>0.20546439943359551</v>
       </c>
       <c r="R4" s="21">
         <f t="shared" ref="R4:R10" ca="1" si="15">RANDBETWEEN(1000,9999)</f>
-        <v>7462</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1527,11 +1566,11 @@
       </c>
       <c r="Q5" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.17839651414444468</v>
+        <v>0.18027926433163421</v>
       </c>
       <c r="R5" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>2552</v>
+        <v>8666</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1599,11 +1638,11 @@
       </c>
       <c r="Q6" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.15898656482926321</v>
+        <v>0.5800268124659097</v>
       </c>
       <c r="R6" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>6738</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1671,11 +1710,11 @@
       </c>
       <c r="Q7" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.85981117844038923</v>
+        <v>0.50979355468534504</v>
       </c>
       <c r="R7" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>9339</v>
+        <v>7751</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1743,11 +1782,11 @@
       </c>
       <c r="Q8" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.47021275594738077</v>
+        <v>0.36680329558310953</v>
       </c>
       <c r="R8" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>6427</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1815,11 +1854,11 @@
       </c>
       <c r="Q9" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.27122719465849066</v>
+        <v>0.12761270558447246</v>
       </c>
       <c r="R9" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>5930</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1887,11 +1926,11 @@
       </c>
       <c r="Q10" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>6.1146620270365215E-2</v>
+        <v>0.18621938465794574</v>
       </c>
       <c r="R10" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>9383</v>
+        <v>6267</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1952,28 +1991,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -1988,16 +2027,16 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -2042,7 +2081,7 @@
       </c>
       <c r="E6" s="3">
         <f ca="1">TODAY()</f>
-        <v>45861</v>
+        <v>45887</v>
       </c>
       <c r="F6">
         <f>YEAR(D6)</f>
@@ -2066,7 +2105,7 @@
       </c>
       <c r="L6">
         <f ca="1">DATEDIF(D6,E6,"D")</f>
-        <v>1097</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -2084,7 +2123,7 @@
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <f ca="1">NOW()</f>
-        <v>45861.464112268521</v>
+        <v>45887.633442361112</v>
       </c>
       <c r="D10" s="3"/>
       <c r="I10" s="20"/>
@@ -2184,7 +2223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -2222,66 +2261,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
     </row>
     <row r="2" spans="1:27" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="47"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="41"/>
     </row>
     <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -2317,7 +2356,7 @@
       <c r="K3" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="35" t="s">
         <v>190</v>
       </c>
       <c r="M3" s="23" t="s">
@@ -2357,7 +2396,7 @@
       <c r="Y3" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="Z3" s="44" t="s">
+      <c r="Z3" s="36" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2450,7 +2489,7 @@
       </c>
       <c r="Z4" t="str">
         <f ca="1">UPPER(CONCATENATE("CUST",LEFT(A4,2),"BR",B4,"LOC",LEFT(C4,3),RANDBETWEEN(1000,9999)))</f>
-        <v>CUST75BRALOCTRI5500</v>
+        <v>CUST75BRALOCTRI4822</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -2502,7 +2541,7 @@
       </c>
       <c r="Z5" t="str">
         <f t="shared" ref="Z5:Z34" ca="1" si="2">UPPER(CONCATENATE("CUST",LEFT(A5,2),"BR",B5,"LOC",LEFT(C5,3),RANDBETWEEN(1000,9999)))</f>
-        <v>CUST22BRCLOCCHE2349</v>
+        <v>CUST22BRCLOCCHE3042</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -2550,7 +2589,7 @@
       </c>
       <c r="Z6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST63BRALOCTRI4058</v>
+        <v>CUST63BRALOCTRI8099</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -2598,7 +2637,7 @@
       </c>
       <c r="Z7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST12BRALOCTRI9418</v>
+        <v>CUST12BRALOCTRI3011</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -2646,7 +2685,7 @@
       </c>
       <c r="Z8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST37BRALOCTRI5607</v>
+        <v>CUST37BRALOCTRI9811</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -2701,7 +2740,7 @@
       </c>
       <c r="Z9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST69BRCLOCCHE6619</v>
+        <v>CUST69BRCLOCCHE5602</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -2749,7 +2788,7 @@
       </c>
       <c r="Z10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST35BRALOCTRI5075</v>
+        <v>CUST35BRALOCTRI5242</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -2797,7 +2836,7 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST31BRCLOCCHE2660</v>
+        <v>CUST31BRCLOCCHE1208</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
@@ -2845,7 +2884,7 @@
       </c>
       <c r="Z12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST66BRALOCTRI1772</v>
+        <v>CUST66BRALOCTRI2340</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
@@ -2893,7 +2932,7 @@
       </c>
       <c r="Z13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST69BRBLOCKAR9654</v>
+        <v>CUST69BRBLOCKAR7286</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -2941,7 +2980,7 @@
       </c>
       <c r="Z14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST35BRBLOCKAR4172</v>
+        <v>CUST35BRBLOCKAR2229</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
@@ -2989,7 +3028,7 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST52BRBLOCKAR2753</v>
+        <v>CUST52BRBLOCKAR3344</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -3037,7 +3076,7 @@
       </c>
       <c r="Z16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST36BRALOCTRI7736</v>
+        <v>CUST36BRALOCTRI2964</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -3085,7 +3124,7 @@
       </c>
       <c r="Z17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST25BRALOCTRI1666</v>
+        <v>CUST25BRALOCTRI9593</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -3133,7 +3172,7 @@
       </c>
       <c r="Z18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST82BRALOCTRI7811</v>
+        <v>CUST82BRALOCTRI7610</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -3181,7 +3220,7 @@
       </c>
       <c r="Z19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST29BRBLOCKAR7249</v>
+        <v>CUST29BRBLOCKAR4488</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -3229,7 +3268,7 @@
       </c>
       <c r="Z20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST65BRALOCTRI8257</v>
+        <v>CUST65BRALOCTRI7116</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -3277,7 +3316,7 @@
       </c>
       <c r="Z21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST76BRALOCTRI4521</v>
+        <v>CUST76BRALOCTRI1880</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -3325,7 +3364,7 @@
       </c>
       <c r="Z22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST32BRALOCTRI8938</v>
+        <v>CUST32BRALOCTRI9684</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -3373,7 +3412,7 @@
       </c>
       <c r="Z23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST31BRBLOCKAR7063</v>
+        <v>CUST31BRBLOCKAR1751</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -3421,7 +3460,7 @@
       </c>
       <c r="Z24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST30BRCLOCCHE2301</v>
+        <v>CUST30BRCLOCCHE5564</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -3469,7 +3508,7 @@
       </c>
       <c r="Z25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST37BRBLOCKAR5067</v>
+        <v>CUST37BRBLOCKAR1425</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -3517,7 +3556,7 @@
       </c>
       <c r="Z26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST27BRBLOCKAR4230</v>
+        <v>CUST27BRBLOCKAR1869</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -3565,7 +3604,7 @@
       </c>
       <c r="Z27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST63BRALOCTRI8198</v>
+        <v>CUST63BRALOCTRI6900</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -3613,7 +3652,7 @@
       </c>
       <c r="Z28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST54BRALOCTRI9986</v>
+        <v>CUST54BRALOCTRI6481</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -3661,7 +3700,7 @@
       </c>
       <c r="Z29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST22BRALOCTRI3176</v>
+        <v>CUST22BRALOCTRI9273</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -3709,7 +3748,7 @@
       </c>
       <c r="Z30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST64BRBLOCKAR1395</v>
+        <v>CUST64BRBLOCKAR2574</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -3757,7 +3796,7 @@
       </c>
       <c r="Z31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST18BRALOCTRI5552</v>
+        <v>CUST18BRALOCTRI2934</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -3805,7 +3844,7 @@
       </c>
       <c r="Z32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST14BRBLOCKAR2849</v>
+        <v>CUST14BRBLOCKAR9979</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
@@ -3853,7 +3892,7 @@
       </c>
       <c r="Z33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST84BRALOCTRI2363</v>
+        <v>CUST84BRALOCTRI6151</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
@@ -3901,7 +3940,7 @@
       </c>
       <c r="Z34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUST87BRBLOCKAR1055</v>
+        <v>CUST87BRBLOCKAR6552</v>
       </c>
     </row>
   </sheetData>
@@ -3916,467 +3955,476 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:C8"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="61" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
-    <col min="7" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="61" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1"/>
+    <col min="8" max="9" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="S1" s="11" t="s">
+      <c r="R1" s="8"/>
+      <c r="T1" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="1:21" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42"/>
+      <c r="B2" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
+      <c r="P2" s="7"/>
       <c r="Q2" s="8"/>
-      <c r="S2" s="11" t="s">
+      <c r="R2" s="8"/>
+      <c r="T2" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="9" t="s">
+    <row r="3" spans="1:21" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="T3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>40</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="12">
+        <v>33300</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="13" t="str">
+        <f>IF(B4="ravi","this is ravi","this is not ravi")</f>
+        <v>this is not ravi</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="13" t="b">
+        <f>OR(A4&gt;10, C4&lt;30)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="13" t="b">
+        <f>AND(A4&gt;10, C4&lt;30)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="13" t="str">
-        <f>IF(A4&gt;20, "true", "Fasle")</f>
-        <v>true</v>
-      </c>
-      <c r="E4" s="14" t="b">
-        <f>AND(A4&gt;10, B4&lt;30)</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="13" t="b">
-        <f>OR(A4&gt;10, B4&lt;30)</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="13" t="b">
-        <f>AND(A4&gt;10, B4&lt;30)</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="13" t="b">
+      <c r="I4" s="13" t="b">
         <f>NOT(A4&gt;15)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="13" t="str">
-        <f>IFERROR(A4/B4, "Division by ZeroERROR")</f>
-        <v>Division by ZeroERROR</v>
-      </c>
-      <c r="J4" s="13" t="e">
-        <f ca="1">IFS(A4&gt;30, "Above 30", B4&gt;20, "Above 20", A5&gt;10, "Above 10")</f>
+      <c r="J4" s="13" t="str">
+        <f>IFERROR(22/"x","cannot divide by letters")</f>
+        <v>cannot divide by letters</v>
+      </c>
+      <c r="K4" s="13" t="e">
+        <f ca="1">IFS(A4&gt;30, "Above 30", C4&gt;20, "Above 20", A5&gt;10, "Above 10")</f>
         <v>#NAME?</v>
       </c>
-      <c r="K4" s="13" t="e">
+      <c r="L4" s="13" t="e">
         <f ca="1">_xlfn.SWITCH("A", "A", "Category A", "B", "Category B", "Unknown")</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="13" t="e">
-        <f ca="1">_xludf.XOR(D3&gt;10, F6&lt;30)</f>
+      <c r="M4" s="13" t="e">
+        <f ca="1">_xludf.XOR(E3&gt;10, G6&lt;30)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M4" s="13" t="b">
+      <c r="N4" s="13" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="N4" s="13" t="b">
+      <c r="O4" s="13" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="O4" s="13" t="str">
+      <c r="P4" s="13" t="str">
         <f>IF(A4&gt;0,"A value is greater than zero", "A value is no greater")</f>
         <v>A value is greater than zero</v>
       </c>
-      <c r="P4" s="12">
-        <f>SUMIF(C4:C8,"A",A4:A8)</f>
-        <v>120</v>
-      </c>
       <c r="Q4" s="12">
-        <f>SUMIFS(A4:A8,C4:C8,"A",B4:B8,0)</f>
+        <f>SUMIF(D4:D8,"A",A4:A8)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="12">
+        <f>SUMIFS(A4:A8,D4:D8,"A",C4:C8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="S4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T4" s="11" t="s">
+      <c r="U4" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>55</v>
       </c>
-      <c r="B5" s="12">
-        <v>25</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="13" t="str">
-        <f>IF(A5&gt;20, IF(C5="A","True","False"), "Less or equal to 20")</f>
-        <v>False</v>
-      </c>
-      <c r="E5" s="14" t="b">
-        <f t="shared" ref="E5:E8" si="0">AND(A5&gt;10, B5&lt;30)</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="13" t="b">
-        <f>OR(A5&lt;10, B5&gt;30)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="13"/>
+      <c r="B5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f>IF(C5&gt;25000,"paid above 25000rs", "not paid above 25000rs")</f>
+        <v>not paid above 25000rs</v>
+      </c>
+      <c r="F5" s="14" t="str">
+        <f>IF(AND(B5="ravi",C5&gt;25000),"yes he is raju and he paid above 25000rs", "no he is not")</f>
+        <v>no he is not</v>
+      </c>
+      <c r="G5" s="14" t="str">
+        <f>IF(OR(C5="ravi",D5&gt;25000),"yes he is raju and he paid above 25000rs", "no he is not")</f>
+        <v>yes he is raju and he paid above 25000rs</v>
+      </c>
       <c r="H5" s="13"/>
-      <c r="I5" s="13">
-        <f>IFERROR(A5/B5, "Error")</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J5" s="13"/>
+      <c r="I5" s="14" t="str">
+        <f>IF(NOT(AND(E5="ravi",F5&gt;25000)),"yes he is raju and he paid above 25000rs", "no he is not")</f>
+        <v>yes he is raju and he paid above 25000rs</v>
+      </c>
+      <c r="J5" s="13">
+        <f>IFERROR(A5/C5, "Error")</f>
+        <v>2.75E-2</v>
+      </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13" t="str">
+      <c r="M5" s="13"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13" t="str">
         <f>IF(A5&gt;30,"A value is greater than given", "A value is no greater than given")</f>
         <v>A value is greater than given</v>
       </c>
-      <c r="P5" s="12">
-        <f t="shared" ref="P5:P8" si="1">SUMIF(C5:C9,"A",A5:A9)</f>
-        <v>80</v>
-      </c>
       <c r="Q5" s="12">
-        <f t="shared" ref="Q5:Q8" si="2">SUMIFS(A5:A9,C5:C9,"A",B5:B9,0)</f>
-        <v>30</v>
-      </c>
-      <c r="S5" s="11" t="s">
+        <f>SUMIF(D5:D9,"A",A5:A9)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="12">
+        <f>SUMIFS(A5:A9,D5:D9,"A",C5:C9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>30</v>
       </c>
-      <c r="B6" s="12">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="13" t="str">
-        <f>IF(A6&gt;20, "Greater than 20", "Less or equal to 20")</f>
-        <v>Greater than 20</v>
-      </c>
-      <c r="E6" s="14" t="b">
-        <f t="shared" si="0"/>
+      <c r="B6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="12">
+        <v>23400</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="13" t="str">
+        <f>IF(B6="raju",CONCATENATE("raju  : ",C6),IF(B6="ragav",CONCATENATE("Ragav : ",C6),IF(B6="ram",CONCATENATE("Ram : ",C6),B6)))</f>
+        <v>raju  : 23400</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="13" t="b">
+        <f>OR(A6&gt;10, C6&lt;30)</f>
         <v>1</v>
       </c>
-      <c r="F6" s="13" t="b">
-        <f t="shared" ref="F6:F8" si="3">OR(A6&gt;10, B6&lt;30)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="13" t="str">
-        <f>IFERROR(A6/B6, "Error")</f>
-        <v>Error</v>
-      </c>
-      <c r="J6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13">
+        <f>IFERROR(A6/C6, "Error")</f>
+        <v>1.2820512820512821E-3</v>
+      </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
-      <c r="O6" s="13" t="str">
-        <f>IF(A6&gt;0,C6, "A value is no greater than given")</f>
-        <v>A</v>
-      </c>
-      <c r="P6" s="12">
-        <f t="shared" si="1"/>
-        <v>80</v>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13" t="str">
+        <f>IF(A6&gt;0,D6, "A value is no greater than given")</f>
+        <v>java</v>
       </c>
       <c r="Q6" s="12">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="S6" s="11" t="s">
+        <f>SUMIF(D6:D10,"A",A6:A10)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="12">
+        <f>SUMIFS(A6:A10,D6:D10,"A",C6:C10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="U6" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>40</v>
       </c>
-      <c r="B7" s="12">
-        <v>45</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="13" t="str">
-        <f>IF(A7&gt;20, "Greater than 20", "Less or equal to 20")</f>
-        <v>Greater than 20</v>
-      </c>
-      <c r="E7" s="14" t="b">
-        <f>AND(A7&gt;10, B7&lt;30)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="13" t="b">
-        <f t="shared" si="3"/>
+      <c r="B7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="12">
+        <v>24570</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" s="13" t="str">
+        <f>IF(B7="raju",CONCATENATE("raju  : ",C7),IF(B7="ragav",CONCATENATE("Ragav : ",C7),IF(B7="ram",CONCATENATE("Ram : ",C7),B7)))</f>
+        <v>Ram : 24570</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="13" t="b">
+        <f>OR(A7&gt;10, C7&lt;30)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13">
-        <f>IFERROR(A7/B7, "Error")</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="J7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13">
+        <f>IFERROR(A7/C7, "Error")</f>
+        <v>1.6280016280016279E-3</v>
+      </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="13"/>
-      <c r="P7" s="12">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
+      <c r="P7" s="13"/>
       <c r="Q7" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="Q7:Q8" si="0">SUMIF(D7:D11,"A",B7:B11)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="R7" s="12">
+        <f t="shared" ref="R7:R8" si="1">SUMIFS(B7:B11,D7:D11,"A",C7:C11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="T7" s="11" t="s">
+      <c r="U7" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>50</v>
       </c>
-      <c r="B8" s="12">
-        <v>55</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="13" t="str">
-        <f>IF(AND(A8&gt;10, B8&lt;30), C8, "Less or equal to 20")</f>
-        <v>Less or equal to 20</v>
-      </c>
-      <c r="E8" s="14" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="13" t="b">
-        <f t="shared" si="3"/>
+      <c r="B8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="12">
+        <v>33300</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="13" t="str">
+        <f t="shared" ref="E8" si="2">IF(B8="raju",CONCATENATE("raju  : ",C8),IF(B8="ragav",CONCATENATE("Ragav : ",C8),IF(B8="ram",CONCATENATE("Ram : ",C8),B8)))</f>
+        <v>Ragav : 33300</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="13" t="b">
+        <f>OR(A8&gt;10, C8&lt;30)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="13">
-        <f>IFERROR(A8/B8, "Error")</f>
-        <v>0.90909090909090906</v>
-      </c>
-      <c r="J8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13">
+        <f>IFERROR(A8/C8, "Error")</f>
+        <v>1.5015015015015015E-3</v>
+      </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="12">
+      <c r="P8" s="13"/>
+      <c r="Q8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="12">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="Q8" s="12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S8" s="11" t="s">
+      <c r="T8" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="U8" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -4387,21 +4435,21 @@
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="17"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
-      <c r="S9" s="11" t="s">
+      <c r="R9" s="12"/>
+      <c r="T9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="U9" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -4417,32 +4465,40 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
-      <c r="S10" s="11" t="s">
+      <c r="R10" s="12"/>
+      <c r="T10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="T10" s="11" t="s">
+      <c r="U10" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="S11" s="11" t="s">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T11" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T11" s="11" t="s">
+      <c r="U11" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T14" t="b">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
+        <f>CONCATENATE(C8,"  ",D8,"  ",B8)</f>
+        <v>33300  java  ragav</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U14" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4476,58 +4532,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
@@ -4543,9 +4599,9 @@
       <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="23" t="s">
         <v>114</v>
       </c>
@@ -4745,10 +4801,10 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="44"/>
       <c r="C16">
         <v>1</v>
       </c>
@@ -4770,10 +4826,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="44"/>
       <c r="C17">
         <v>1</v>
       </c>
@@ -4827,51 +4883,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
@@ -4880,17 +4936,17 @@
       <c r="T2" s="22"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5141,42 +5197,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">

</xml_diff>